<commit_message>
agregando intervalo y frecuencia observada prueba chicuadrada
</commit_message>
<xml_diff>
--- a/reportes/file02.xlsx
+++ b/reportes/file02.xlsx
@@ -395,7 +395,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>32.852335678516</v>
+        <v>NAN</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -403,25 +403,25 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>8.906516481989</v>
+        <v>NAN</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <f>B2/(12*20)</f>
-        <v>0.13688473199382</v>
+      <c r="B4" t="str">
+        <f>B2/(12*500)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <f>B3/(12*20)</f>
-        <v>0.037110485341621</v>
+      <c r="B5" t="str">
+        <f>B3/(12*500)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -429,7 +429,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.092190469973684</v>
+        <v>0.098176176523286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implementacion final prueba chi cuadrada
</commit_message>
<xml_diff>
--- a/reportes/file02.xlsx
+++ b/reportes/file02.xlsx
@@ -395,7 +395,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>NAN</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -403,25 +403,25 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>NAN</v>
+        <v>73.361080202582</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="str">
-        <f>B2/(12*500)</f>
-        <v>0</v>
+      <c r="B4">
+        <f>B2/(12*100)</f>
+        <v>0.083333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="str">
-        <f>B3/(12*500)</f>
-        <v>0</v>
+      <c r="B5">
+        <f>B3/(12*100)</f>
+        <v>0.061134233502152</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -429,7 +429,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.098176176523286</v>
+        <v>0.081194294852525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
comprobacion prueba chi cuadrada implementada
</commit_message>
<xml_diff>
--- a/reportes/file02.xlsx
+++ b/reportes/file02.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>FORMULA</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>var</t>
+  </si>
+  <si>
+    <t>tablaXa,n</t>
   </si>
 </sst>
 </file>
@@ -374,7 +377,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,7 +432,15 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.081194294852525</v>
+        <v>0.065599199873737</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>16.918977604633</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregando nuevas columnas a las validaciones
</commit_message>
<xml_diff>
--- a/reportes/file02.xlsx
+++ b/reportes/file02.xlsx
@@ -398,7 +398,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>NAN</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -406,25 +406,25 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>73.361080202582</v>
+        <v>NAN</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <f>B2/(12*100)</f>
-        <v>0.083333333333333</v>
+      <c r="B4" t="str">
+        <f>B2/(12*1000)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <f>B3/(12*100)</f>
-        <v>0.061134233502152</v>
+      <c r="B5" t="str">
+        <f>B3/(12*1000)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -432,7 +432,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.065599199873737</v>
+        <v>0.069217483891251</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -440,7 +440,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>16.918977604633</v>
+        <v>43.773064159559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
activo y desactivo btn descargar
</commit_message>
<xml_diff>
--- a/reportes/file02.xlsx
+++ b/reportes/file02.xlsx
@@ -398,7 +398,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>NAN</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -406,25 +406,25 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>NAN</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="str">
-        <f>B2/(12*1000)</f>
-        <v>0</v>
+      <c r="B4">
+        <f>B2/(12*150)</f>
+        <v>0.055555555555556</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="str">
-        <f>B3/(12*1000)</f>
-        <v>0</v>
+      <c r="B5">
+        <f>B3/(12*150)</f>
+        <v>0.055555555555556</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -432,7 +432,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.086037811351351</v>
+        <v>0.096541412416107</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -440,7 +440,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>43.773064159559</v>
+        <v>19.675137572927</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregando boton regarcar pagina
</commit_message>
<xml_diff>
--- a/reportes/file02.xlsx
+++ b/reportes/file02.xlsx
@@ -398,7 +398,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>NAN</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -406,25 +406,25 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>NAN</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <f>B2/(12*150)</f>
-        <v>0.055555555555556</v>
+      <c r="B4" t="str">
+        <f>B2/(12*1523)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <f>B3/(12*150)</f>
-        <v>0.055555555555556</v>
+      <c r="B5" t="str">
+        <f>B3/(12*1523)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -432,7 +432,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.096541412416107</v>
+        <v>0.084400690052562</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -440,7 +440,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>19.675137572927</v>
+        <v>53.384528124401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
eliminado problema de desborde offset en prueba de uniformidad
</commit_message>
<xml_diff>
--- a/reportes/file02.xlsx
+++ b/reportes/file02.xlsx
@@ -398,7 +398,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>NAN</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -406,25 +406,25 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>NAN</v>
+        <v>73.361080202582</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="str">
-        <f>B2/(12*1523)</f>
-        <v>0</v>
+      <c r="B4">
+        <f>B2/(12*100)</f>
+        <v>0.083333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="str">
-        <f>B3/(12*1523)</f>
-        <v>0</v>
+      <c r="B5">
+        <f>B3/(12*100)</f>
+        <v>0.061134233502152</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -432,7 +432,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.084400690052562</v>
+        <v>0.086562964848485</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -440,7 +440,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>53.384528124401</v>
+        <v>16.918977604633</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregando reporte de excel
</commit_message>
<xml_diff>
--- a/reportes/file02.xlsx
+++ b/reportes/file02.xlsx
@@ -15,32 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
-  <si>
-    <t>FORMULA</t>
-  </si>
-  <si>
-    <t>VALOR</t>
-  </si>
-  <si>
-    <t>a/2</t>
-  </si>
-  <si>
-    <t>1-(a/2)</t>
-  </si>
-  <si>
-    <t>LI</t>
-  </si>
-  <si>
-    <t>LS</t>
-  </si>
-  <si>
-    <t>var</t>
-  </si>
-  <si>
-    <t>tablaXa,n</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,73 +352,14 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>73.361080202582</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <f>B2/(12*100)</f>
-        <v>0.083333333333333</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <f>B3/(12*100)</f>
-        <v>0.061134233502152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>0.086562964848485</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>16.918977604633</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
mejora parte sobre la aplicación
</commit_message>
<xml_diff>
--- a/reportes/file02.xlsx
+++ b/reportes/file02.xlsx
@@ -352,14 +352,490 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1">
+        <v>0.6298</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>0.2393</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>0.6693</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
+        <v>0.8257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5">
+        <v>0.0668</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <v>0.374</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <v>0.4895</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>0.0524</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>0.4311</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10">
+        <v>0.2284</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11">
+        <v>0.9556</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12">
+        <v>0.5726</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13">
+        <v>0.4938</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14">
+        <v>0.334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15">
+        <v>0.8703</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16">
+        <v>0.9872</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>0.6418</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <v>0.025</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19">
+        <v>0.637</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20">
+        <v>0.7107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21">
+        <v>0.5366</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22">
+        <v>0.1365</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23">
+        <v>0.938</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24">
+        <v>0.4202</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25">
+        <v>0.5146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26">
+        <v>0.696</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27">
+        <v>0.574</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28">
+        <v>0.5855</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29">
+        <v>0.3385</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30">
+        <v>0.1649</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31">
+        <v>0.7976</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32">
+        <v>0.2268</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33">
+        <v>0.8508</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34">
+        <v>0.7103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35">
+        <v>0.5104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36">
+        <v>0.4209</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37">
+        <v>0.5605</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38">
+        <v>0.7015</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39">
+        <v>0.9342</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40">
+        <v>0.1714</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41">
+        <v>0.2232</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42">
+        <v>0.6151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43">
+        <v>0.2767</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44">
+        <v>0.1183</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45">
+        <v>0.7462</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46">
+        <v>0.8611</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47">
+        <v>0.3848</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48">
+        <v>0.1967</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49">
+        <v>0.8799</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50">
+        <v>0.6158</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51">
+        <v>0.3225</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52">
+        <v>0.1173</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53">
+        <v>0.6808</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54">
+        <v>0.5787</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55">
+        <v>0.8932</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56">
+        <v>0.4867</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57">
+        <v>0.8691</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58">
+        <v>0.9086</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59">
+        <v>0.4951</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60">
+        <v>0.4191</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61">
+        <v>0.4426</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62">
+        <v>0.9814</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63">
+        <v>0.262</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64">
+        <v>0.1557</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65">
+        <v>0.1952</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66">
+        <v>0.7816</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67">
+        <v>0.1791</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68">
+        <v>0.7274</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69">
+        <v>0.6301</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70">
+        <v>0.2589</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71">
+        <v>0.9527</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72">
+        <v>0.3827</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73">
+        <v>0.0591</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74">
+        <v>0.8698</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75">
+        <v>0.9545</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76">
+        <v>0.5006</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77">
+        <v>0.7792</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79">
+        <v>0.4405</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80">
+        <v>0.8439</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81">
+        <v>0.2585</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82">
+        <v>0.9265</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83">
+        <v>0.6672</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84">
+        <v>0.6882</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85">
+        <v>0.0633</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86">
+        <v>0.1448</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87">
+        <v>0.4815</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88">
+        <v>0.5286</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89">
+        <v>0.6127</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90">
+        <v>0.1195</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91">
+        <v>0.8248</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92">
+        <v>0.0079</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93">
+        <v>0.1729</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94">
+        <v>0.3214</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95">
+        <v>0.0452</v>
+      </c>
+    </row>
+  </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>